<commit_message>
Created page objects, feature file and steps for View/Edit members
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/translation.xlsx
+++ b/src/test/resources/inputFiles/translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t xml:space="preserve">BaseToken</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">View/Edit Visitors List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Memberships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Members</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -189,6 +195,34 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
This commit includes view palms report.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/translation.xlsx
+++ b/src/test/resources/inputFiles/translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t xml:space="preserve">BaseToken</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">View/Edit Region Business Rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter One to Ones</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -277,6 +280,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Completed the view palms summary feature.This has all the pageobjects and steps.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/translation.xlsx
+++ b/src/test/resources/inputFiles/translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
   <si>
     <t xml:space="preserve">BaseToken</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t xml:space="preserve">Enter One to Ones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View PALMS Summary</t>
   </si>
 </sst>
 </file>
@@ -156,7 +162,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -294,6 +300,34 @@
         <v>11</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
EnterPalms feature completed, includes feature file, page objects and step definition.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/translation.xlsx
+++ b/src/test/resources/inputFiles/translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
   <si>
     <t xml:space="preserve">BaseToken</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">View PALMS Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter PALMS</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -328,6 +331,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
verify mass email feature completed.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/translation.xlsx
+++ b/src/test/resources/inputFiles/translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
   <si>
     <t xml:space="preserve">BaseToken</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t xml:space="preserve">View / Allocate Roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Members</t>
   </si>
 </sst>
 </file>
@@ -174,10 +180,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,6 +402,34 @@
         <v>17</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>